<commit_message>
Added http to report, updated http values in results, and modified httpClient to automate running of all files the correct number of times
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rishabgu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Documents\NC_State\Graduate School\Spring 2023\CSC591 - IoT\Homeworks\Homework 2\IoT-hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DBB6D5-2470-4875-9876-6AA9DD57B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A355F-0C80-4321-A3D6-62F382B14786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7470" yWindow="2085" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,98 +428,98 @@
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -839,19 +839,19 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="17" width="9.08984375" customWidth="1"/>
+    <col min="14" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
@@ -869,7 +869,7 @@
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="32" t="s">
         <v>2</v>
       </c>
@@ -899,7 +899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -978,7 +978,7 @@
         <v>1.000002616238</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>1.0000029038288101</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1060,45 +1060,45 @@
         <v>1.0132000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="22">
-        <v>4623459.3660000004</v>
+        <v>566.24</v>
       </c>
       <c r="C7" s="23">
-        <v>17470.572</v>
+        <v>36.14</v>
       </c>
       <c r="D7" s="23">
-        <v>141065.92600000001</v>
+        <v>55946.98</v>
       </c>
       <c r="E7" s="23">
-        <v>349456.18800000002</v>
+        <v>3105.75</v>
       </c>
       <c r="F7" s="23">
-        <v>10355.538</v>
+        <v>47887.27</v>
       </c>
       <c r="G7" s="23">
-        <v>10136.509</v>
+        <v>5395.2</v>
       </c>
       <c r="H7" s="23">
-        <v>5128.3100000000004</v>
+        <v>1036.96</v>
       </c>
       <c r="I7" s="24">
-        <v>4180.0749999999998</v>
+        <v>4.67</v>
       </c>
       <c r="J7" s="25">
-        <v>579348967.96899998</v>
+        <v>3.0099900000000002</v>
       </c>
       <c r="K7" s="23">
-        <v>10320383.302999999</v>
+        <v>1.02725</v>
       </c>
       <c r="L7" s="23">
-        <v>2565.1999999999998</v>
+        <v>1.0081899999999999</v>
       </c>
       <c r="M7" s="24">
-        <v>139.67699999999999</v>
+        <v>1.0158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HTTP results XLSX file
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Documents\NC_State\Graduate School\Spring 2023\CSC591 - IoT\Homeworks\Homework 2\IoT-hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2A355F-0C80-4321-A3D6-62F382B14786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB4A73-43F4-436A-A8CD-C85068284BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="2085" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2085" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -839,7 +839,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,40 +1065,40 @@
         <v>11</v>
       </c>
       <c r="B7" s="22">
-        <v>566.24</v>
+        <v>57.23</v>
       </c>
       <c r="C7" s="23">
-        <v>36.14</v>
+        <v>10.1</v>
       </c>
       <c r="D7" s="23">
-        <v>55946.98</v>
+        <v>2791.76</v>
       </c>
       <c r="E7" s="23">
-        <v>3105.75</v>
+        <v>380.36</v>
       </c>
       <c r="F7" s="23">
-        <v>47887.27</v>
+        <v>56156.39</v>
       </c>
       <c r="G7" s="23">
-        <v>5395.2</v>
+        <v>9694.0499999999993</v>
       </c>
       <c r="H7" s="23">
-        <v>1036.96</v>
+        <v>67710.94</v>
       </c>
       <c r="I7" s="24">
-        <v>4.67</v>
+        <v>7408.72</v>
       </c>
       <c r="J7" s="25">
         <v>3.0099900000000002</v>
       </c>
       <c r="K7" s="23">
-        <v>1.02725</v>
+        <v>1.0198199999999999</v>
       </c>
       <c r="L7" s="23">
-        <v>1.0081899999999999</v>
+        <v>1.0002</v>
       </c>
       <c r="M7" s="24">
-        <v>1.0158</v>
+        <v>1.0000199999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update report and fix decimal point in results
</commit_message>
<xml_diff>
--- a/Results File.xlsx
+++ b/Results File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Documents\NC_State\Graduate School\Spring 2023\CSC591 - IoT\Homeworks\Homework 2\IoT-hw2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FB4A73-43F4-436A-A8CD-C85068284BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B848F0-677F-41FD-B456-D382210C51F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2085" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -839,7 +839,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,7 @@
         <v>11232.82</v>
       </c>
       <c r="H5" s="18">
-        <v>43415.610999999997</v>
+        <v>43415.61</v>
       </c>
       <c r="I5" s="19">
         <v>10142.61</v>

</xml_diff>